<commit_message>
Added new data and fixed ordering of groups.
</commit_message>
<xml_diff>
--- a/data/nl/outcome_table.xlsx
+++ b/data/nl/outcome_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveeur-my.sharepoint.com/personal/557513dp_eur_nl/Documents/Kansenlab/kenniscentrumongelijkheid-main/data/nl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kenniscentrumongelijkheid/data/nl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{ECE2F296-FD9F-4090-85D3-4D2D191914E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17B30E09-CDA8-8D4D-95BE-11B40440D7C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F9AFF0-C167-D64A-A5D6-CC66067B61AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="6" r:id="rId1"/>
@@ -132,7 +132,7 @@
     <t>zijn de gemiddelde totale zorgkosten, vergoed vanuit de Zorgverzekeringswet, van 16-jarigen in het jaar dat zij 16 werden.</t>
   </si>
   <si>
-    <t>c21_young_parent</t>
+    <t>c21_young_parents</t>
   </si>
   <si>
     <t>Jong ouderschap</t>
@@ -141,15 +141,18 @@
     <t>is het percentage 21-jarigen dat een kind kreeg voor de 20e verjaardag.</t>
   </si>
   <si>
+    <t>21-jarigen</t>
+  </si>
+  <si>
+    <t>c30_total_health_costs</t>
+  </si>
+  <si>
+    <t>zijn de gemiddelde totale zorgkosten van 35-jarigen, vergoed vanuit de Zorgverzekeringswet, in het jaar dat zij 35 werden.</t>
+  </si>
+  <si>
     <t>35-jarigen</t>
   </si>
   <si>
-    <t>c30_total_health_costs</t>
-  </si>
-  <si>
-    <t>zijn de gemiddelde totale zorgkosten van 35-jarigen, vergoed vanuit de Zorgverzekeringswet, in het jaar dat zij 35 werden.</t>
-  </si>
-  <si>
     <t>c30_hospital</t>
   </si>
   <si>
@@ -322,9 +325,6 @@
   </si>
   <si>
     <t>is het percentage 21-jarigen dat een startkwalificatie heeft behaald (havo, vwo, of mbo niveau 2 of hoger).</t>
-  </si>
-  <si>
-    <t>21-jarigen</t>
   </si>
   <si>
     <t>c21_hbo_followed</t>
@@ -564,15 +564,12 @@
     <t>years</t>
   </si>
   <si>
-    <t>c35_age_left_parents</t>
+    <t>c30_age_left_parents</t>
   </si>
   <si>
     <t>Leeftijd waarop ouderlijk huis is verlaten</t>
   </si>
   <si>
-    <t>is de gemiddelde leeftjid waarip 35-jarigen het ouderlijk huis hebben verlaten.</t>
-  </si>
-  <si>
     <t>c30_living_space_pp</t>
   </si>
   <si>
@@ -787,6 +784,9 @@
   </si>
   <si>
     <t>Buitenveldert, Zuidas</t>
+  </si>
+  <si>
+    <t>is de gemiddelde leeftjid waarop 35-jarigen het ouderlijk huis hebben verlaten.</t>
   </si>
 </sst>
 </file>
@@ -841,7 +841,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,6 +872,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -885,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -909,7 +921,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1226,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="128.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1330,7 +1345,7 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1351,7 +1366,7 @@
       <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1371,7 +1386,7 @@
       <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1392,7 +1407,7 @@
       <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1421,8 +1436,8 @@
       <c r="E9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>95</v>
+      <c r="F9" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1442,7 +1457,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G10"/>
     </row>
@@ -1451,19 +1466,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1471,19 +1486,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1491,19 +1506,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1511,19 +1526,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1531,16 +1546,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>21</v>
@@ -1552,16 +1567,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>21</v>
@@ -1573,16 +1588,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>21</v>
@@ -1594,16 +1609,16 @@
         <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>21</v>
@@ -1615,16 +1630,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>21</v>
@@ -1636,16 +1651,16 @@
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>21</v>
@@ -1657,16 +1672,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>21</v>
@@ -1677,16 +1692,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>21</v>
@@ -1698,16 +1713,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>21</v>
@@ -1718,16 +1733,16 @@
         <v>6</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>21</v>
@@ -1739,16 +1754,16 @@
         <v>6</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>21</v>
@@ -1759,16 +1774,16 @@
         <v>6</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>28</v>
@@ -1779,16 +1794,16 @@
         <v>6</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>28</v>
@@ -1799,16 +1814,16 @@
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>28</v>
@@ -1819,19 +1834,19 @@
         <v>6</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1845,13 +1860,13 @@
         <v>97</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>98</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1865,13 +1880,13 @@
         <v>100</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>101</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1885,13 +1900,13 @@
         <v>103</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>104</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G32"/>
     </row>
@@ -1906,174 +1921,174 @@
         <v>106</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>107</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>169</v>
+      <c r="B37" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>170</v>
+        <v>110</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>171</v>
+      <c r="A38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>172</v>
+        <v>110</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>173</v>
+        <v>22</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>175</v>
+        <v>110</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>22</v>
+      <c r="A40" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>109</v>
+        <v>128</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>111</v>
+      <c r="E40" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>113</v>
+        <v>6</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>114</v>
+      <c r="E41" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2081,279 +2096,279 @@
         <v>6</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>110</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>118</v>
+        <v>6</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>110</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>124</v>
+      <c r="E44" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>126</v>
+      <c r="B45" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>144</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>127</v>
+      <c r="E45" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>129</v>
+        <v>22</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>130</v>
+      <c r="E46" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
-        <v>6</v>
+      <c r="A47" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>132</v>
+        <v>149</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>133</v>
+      <c r="E47" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>135</v>
+      <c r="A48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>136</v>
+      <c r="E48" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>138</v>
+      <c r="A49" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>139</v>
+      <c r="E49" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>110</v>
+        <v>159</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>110</v>
+      <c r="A51" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>34</v>
+        <v>163</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>146</v>
+        <v>6</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>148</v>
+        <v>165</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>166</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>151</v>
+      <c r="A53" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>242</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>154</v>
+        <v>170</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>157</v>
+      <c r="A55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2377,7 +2392,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -2385,506 +2400,506 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>